<commit_message>
verificacion previa agregar dispositivo y sesion, agregar datos a tarjetas
</commit_message>
<xml_diff>
--- a/api/db/010825.xlsx
+++ b/api/db/010825.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alienware\Desktop\Proyectos software\EOLO_WEBAPP\api\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B415BDA8-C89D-42BD-A2B1-E5E85822E6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E9D7E3-348B-4CC6-83BC-6E3D154D4994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="16">
   <si>
     <t>sesion_id</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>presion</t>
+  </si>
+  <si>
+    <t>volumen</t>
+  </si>
+  <si>
+    <t>flujo</t>
   </si>
 </sst>
 </file>
@@ -400,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -413,7 +419,7 @@
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -444,8 +450,14 @@
       <c r="J1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -476,8 +488,14 @@
       <c r="J2">
         <v>1050</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="1">
+        <v>200</v>
+      </c>
+      <c r="L2" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -508,8 +526,14 @@
       <c r="J3">
         <v>1050</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="1">
+        <v>200</v>
+      </c>
+      <c r="L3" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -540,8 +564,14 @@
       <c r="J4">
         <v>1050</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="1">
+        <v>200</v>
+      </c>
+      <c r="L4" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -572,8 +602,14 @@
       <c r="J5">
         <v>1050</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="1">
+        <v>200</v>
+      </c>
+      <c r="L5" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -604,8 +640,14 @@
       <c r="J6">
         <v>1050</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="1">
+        <v>200</v>
+      </c>
+      <c r="L6" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -636,8 +678,14 @@
       <c r="J7">
         <v>1050</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="1">
+        <v>200</v>
+      </c>
+      <c r="L7" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -668,8 +716,14 @@
       <c r="J8">
         <v>1050</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="1">
+        <v>200</v>
+      </c>
+      <c r="L8" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -700,8 +754,14 @@
       <c r="J9">
         <v>1050</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="1">
+        <v>200</v>
+      </c>
+      <c r="L9" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -732,8 +792,14 @@
       <c r="J10">
         <v>1050</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="1">
+        <v>200</v>
+      </c>
+      <c r="L10" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -764,8 +830,14 @@
       <c r="J11">
         <v>1050</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="1">
+        <v>200</v>
+      </c>
+      <c r="L11" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -796,8 +868,14 @@
       <c r="J12">
         <v>1050</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="1">
+        <v>200</v>
+      </c>
+      <c r="L12" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -828,8 +906,14 @@
       <c r="J13">
         <v>1050</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="1">
+        <v>200</v>
+      </c>
+      <c r="L13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -860,8 +944,14 @@
       <c r="J14">
         <v>1050</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="1">
+        <v>200</v>
+      </c>
+      <c r="L14" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -892,8 +982,14 @@
       <c r="J15">
         <v>1050</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="1">
+        <v>200</v>
+      </c>
+      <c r="L15" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -924,8 +1020,14 @@
       <c r="J16">
         <v>1050</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="1">
+        <v>200</v>
+      </c>
+      <c r="L16" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -956,8 +1058,14 @@
       <c r="J17">
         <v>1050</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="1">
+        <v>200</v>
+      </c>
+      <c r="L17" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -988,8 +1096,14 @@
       <c r="J18">
         <v>1050</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="1">
+        <v>200</v>
+      </c>
+      <c r="L18" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1020,8 +1134,14 @@
       <c r="J19">
         <v>1050</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="1">
+        <v>200</v>
+      </c>
+      <c r="L19" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1051,6 +1171,12 @@
       </c>
       <c r="J20">
         <v>1050</v>
+      </c>
+      <c r="K20" s="1">
+        <v>200</v>
+      </c>
+      <c r="L20" s="1">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>